<commit_message>
Remove device Name From and change sheet Name
</commit_message>
<xml_diff>
--- a/templates/export/events.xlsx
+++ b/templates/export/events.xlsx
@@ -65,18 +65,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Report type:</t>
   </si>
   <si>
     <t>Events</t>
-  </si>
-  <si>
-    <t>Device:</t>
-  </si>
-  <si>
-    <t>${device.deviceName}</t>
   </si>
   <si>
     <t>Group:</t>
@@ -438,7 +432,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="0" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -491,7 +485,7 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -506,59 +500,6 @@
           <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
         <a:ln w="9360">
-          <a:solidFill>
-            <a:srgbClr val="000000"/>
-          </a:solidFill>
-          <a:miter lim="800000"/>
-        </a:ln>
-      </xdr:spPr>
-      <xdr:style>
-        <a:lnRef idx="0">
-          <a:srgbClr val="000000"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </xdr:style>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>1133280</xdr:colOff>
-      <xdr:row>48</xdr:row>
-      <xdr:rowOff>171000</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="CustomShape 1" hidden="1"/>
-        <xdr:cNvSpPr/>
-      </xdr:nvSpPr>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="0" y="0"/>
-          <a:ext cx="9525000" cy="9525000"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="9525">
           <a:solidFill>
             <a:srgbClr val="000000"/>
           </a:solidFill>
@@ -651,6 +592,59 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="6" name="CustomShape 1" hidden="1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="9525000" cy="9525000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="9525">
+          <a:solidFill>
+            <a:srgbClr val="000000"/>
+          </a:solidFill>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:srgbClr val="000000"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1133280</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>171000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="CustomShape 1" hidden="1"/>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -980,7 +974,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -991,7 +985,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="A4" sqref="A4:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4"/>
@@ -1029,22 +1023,18 @@
       <c r="E3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>3</v>
-      </c>
+      <c r="A4" s="1"/>
+      <c r="B4" s="6"/>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
       <c r="E4" s="7"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -1052,10 +1042,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -1070,42 +1060,42 @@
     </row>
     <row r="8" spans="1:6" ht="29.25" customHeight="1">
       <c r="A8" s="10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B8" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="10" t="s">
+      <c r="E8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="F8" s="10" t="s">
         <v>10</v>
-      </c>
-      <c r="E8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1">
       <c r="A9" s="11" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B9" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="E9" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="11" t="s">
+      <c r="F9" s="13" t="s">
         <v>15</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="F9" s="13" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>